<commit_message>
created data trained practice branch
</commit_message>
<xml_diff>
--- a/Project1-micro-Credit/best-model.xlsx
+++ b/Project1-micro-Credit/best-model.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Model Name</t>
   </si>
@@ -48,6 +49,12 @@
   </si>
   <si>
     <t>SVC</t>
+  </si>
+  <si>
+    <t>Kneighbors</t>
+  </si>
+  <si>
+    <t>MultinomialNB</t>
   </si>
 </sst>
 </file>
@@ -110,11 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
@@ -472,4 +480,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="D2" s="2">
+        <f>B2-C2</f>
+        <v>0.10999999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D7" si="0">B3-C3</f>
+        <v>7.999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000071E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>